<commit_message>
add docs and fix segment fault
</commit_message>
<xml_diff>
--- a/docs/CS163-22APCS1-2-Solo Project-Grading Scheme.xlsx
+++ b/docs/CS163-22APCS1-2-Solo Project-Grading Scheme.xlsx
@@ -443,11 +443,11 @@
   </sheetPr>
   <dimension ref="A1:K991"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A46" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D68" activeCellId="0" sqref="D68"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A14" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D20" activeCellId="0" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="62.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="3" style="0" width="18.88"/>
@@ -777,11 +777,11 @@
       <c r="B20" s="9"/>
       <c r="C20" s="9" t="n">
         <f aca="false">SUM(C22:K180)</f>
-        <v>108</v>
+        <v>118</v>
       </c>
       <c r="D20" s="9" t="n">
         <f aca="false">SUM(D22:L180)</f>
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="E20" s="9"/>
       <c r="F20" s="9"/>
@@ -881,7 +881,7 @@
         <v>1</v>
       </c>
       <c r="D25" s="11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E25" s="11"/>
       <c r="F25" s="11"/>
@@ -923,7 +923,7 @@
         <v>1</v>
       </c>
       <c r="D27" s="11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E27" s="11"/>
       <c r="F27" s="11"/>
@@ -965,7 +965,7 @@
         <v>1</v>
       </c>
       <c r="D29" s="11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E29" s="11"/>
       <c r="F29" s="11"/>
@@ -1064,7 +1064,7 @@
         <v>1</v>
       </c>
       <c r="D34" s="11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E34" s="11"/>
       <c r="F34" s="11"/>
@@ -1095,7 +1095,7 @@
       <c r="J35" s="11"/>
       <c r="K35" s="11"/>
     </row>
-    <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="12" t="n">
         <v>23</v>
       </c>
@@ -1103,7 +1103,9 @@
         <v>35</v>
       </c>
       <c r="C36" s="12"/>
-      <c r="D36" s="11"/>
+      <c r="D36" s="11" t="n">
+        <v>0</v>
+      </c>
       <c r="E36" s="11"/>
       <c r="F36" s="11"/>
       <c r="G36" s="11"/>
@@ -1112,7 +1114,7 @@
       <c r="J36" s="11"/>
       <c r="K36" s="11"/>
     </row>
-    <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="12" t="n">
         <v>24</v>
       </c>
@@ -1120,7 +1122,9 @@
         <v>35</v>
       </c>
       <c r="C37" s="12"/>
-      <c r="D37" s="11"/>
+      <c r="D37" s="11" t="n">
+        <v>0</v>
+      </c>
       <c r="E37" s="11"/>
       <c r="F37" s="11"/>
       <c r="G37" s="11"/>
@@ -1140,7 +1144,7 @@
         <v>1</v>
       </c>
       <c r="D38" s="11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E38" s="11"/>
       <c r="F38" s="11"/>
@@ -1182,7 +1186,7 @@
         <v>1</v>
       </c>
       <c r="D40" s="11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E40" s="11"/>
       <c r="F40" s="11"/>
@@ -1270,7 +1274,7 @@
       <c r="J44" s="11"/>
       <c r="K44" s="11"/>
     </row>
-    <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="11" t="n">
         <v>41</v>
       </c>
@@ -1280,7 +1284,9 @@
       <c r="C45" s="11" t="n">
         <v>1</v>
       </c>
-      <c r="D45" s="11"/>
+      <c r="D45" s="11" t="n">
+        <v>0</v>
+      </c>
       <c r="E45" s="11"/>
       <c r="F45" s="11"/>
       <c r="G45" s="11"/>
@@ -1289,7 +1295,7 @@
       <c r="J45" s="11"/>
       <c r="K45" s="11"/>
     </row>
-    <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="11" t="n">
         <v>42</v>
       </c>
@@ -1299,7 +1305,9 @@
       <c r="C46" s="11" t="n">
         <v>2</v>
       </c>
-      <c r="D46" s="11"/>
+      <c r="D46" s="11" t="n">
+        <v>0</v>
+      </c>
       <c r="E46" s="11"/>
       <c r="F46" s="11"/>
       <c r="G46" s="11"/>
@@ -1308,7 +1316,7 @@
       <c r="J46" s="11"/>
       <c r="K46" s="11"/>
     </row>
-    <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="12" t="n">
         <v>43</v>
       </c>
@@ -1316,7 +1324,9 @@
         <v>35</v>
       </c>
       <c r="C47" s="11"/>
-      <c r="D47" s="11"/>
+      <c r="D47" s="11" t="n">
+        <v>0</v>
+      </c>
       <c r="E47" s="11"/>
       <c r="F47" s="11"/>
       <c r="G47" s="11"/>
@@ -1325,7 +1335,7 @@
       <c r="J47" s="11"/>
       <c r="K47" s="11"/>
     </row>
-    <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="12" t="n">
         <v>44</v>
       </c>
@@ -1333,7 +1343,9 @@
         <v>35</v>
       </c>
       <c r="C48" s="11"/>
-      <c r="D48" s="11"/>
+      <c r="D48" s="11" t="n">
+        <v>0</v>
+      </c>
       <c r="E48" s="11"/>
       <c r="F48" s="11"/>
       <c r="G48" s="11"/>
@@ -1342,7 +1354,7 @@
       <c r="J48" s="11"/>
       <c r="K48" s="11"/>
     </row>
-    <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="11" t="n">
         <v>45</v>
       </c>
@@ -1352,7 +1364,9 @@
       <c r="C49" s="11" t="n">
         <v>1</v>
       </c>
-      <c r="D49" s="11"/>
+      <c r="D49" s="11" t="n">
+        <v>0</v>
+      </c>
       <c r="E49" s="11"/>
       <c r="F49" s="11"/>
       <c r="G49" s="11"/>
@@ -1361,7 +1375,7 @@
       <c r="J49" s="11"/>
       <c r="K49" s="11"/>
     </row>
-    <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="11" t="n">
         <v>46</v>
       </c>
@@ -1371,7 +1385,9 @@
       <c r="C50" s="11" t="n">
         <v>2</v>
       </c>
-      <c r="D50" s="11"/>
+      <c r="D50" s="11" t="n">
+        <v>0</v>
+      </c>
       <c r="E50" s="11"/>
       <c r="F50" s="11"/>
       <c r="G50" s="11"/>
@@ -1380,7 +1396,7 @@
       <c r="J50" s="11"/>
       <c r="K50" s="11"/>
     </row>
-    <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="11" t="n">
         <v>47</v>
       </c>
@@ -1390,7 +1406,9 @@
       <c r="C51" s="11" t="n">
         <v>1</v>
       </c>
-      <c r="D51" s="11"/>
+      <c r="D51" s="11" t="n">
+        <v>0</v>
+      </c>
       <c r="E51" s="11"/>
       <c r="F51" s="11"/>
       <c r="G51" s="11"/>
@@ -1399,7 +1417,7 @@
       <c r="J51" s="11"/>
       <c r="K51" s="11"/>
     </row>
-    <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="11" t="n">
         <v>48</v>
       </c>
@@ -1409,7 +1427,9 @@
       <c r="C52" s="11" t="n">
         <v>1</v>
       </c>
-      <c r="D52" s="11"/>
+      <c r="D52" s="11" t="n">
+        <v>0</v>
+      </c>
       <c r="E52" s="11"/>
       <c r="F52" s="11"/>
       <c r="G52" s="11"/>
@@ -1486,7 +1506,7 @@
         <v>1</v>
       </c>
       <c r="D56" s="11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E56" s="11"/>
       <c r="F56" s="11"/>
@@ -1528,7 +1548,7 @@
         <v>1</v>
       </c>
       <c r="D58" s="11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E58" s="11"/>
       <c r="F58" s="11"/>
@@ -1669,7 +1689,7 @@
         <v>1</v>
       </c>
       <c r="D65" s="11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E65" s="11"/>
       <c r="F65" s="11"/>
@@ -1711,7 +1731,7 @@
         <v>1</v>
       </c>
       <c r="D67" s="11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E67" s="11"/>
       <c r="F67" s="11"/>
@@ -1753,7 +1773,7 @@
         <v>1</v>
       </c>
       <c r="D69" s="11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E69" s="11"/>
       <c r="F69" s="11"/>
@@ -2142,7 +2162,7 @@
       <c r="J88" s="11"/>
       <c r="K88" s="11"/>
     </row>
-    <row r="89" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="12" t="n">
         <v>80</v>
       </c>
@@ -2172,7 +2192,7 @@
         <v>1</v>
       </c>
       <c r="D90" s="11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E90" s="11"/>
       <c r="F90" s="11"/>

</xml_diff>